<commit_message>
int simulate ok, correct the data conflit, simulate ok
</commit_message>
<xml_diff>
--- a/docs/inst_list_type.xlsx
+++ b/docs/inst_list_type.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CPU\mcpu\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="120">
   <si>
     <t>imm如果备注没有说明均为sgi(imm)</t>
   </si>
@@ -262,9 +267,6 @@
     <t>lw_sp</t>
   </si>
   <si>
-    <t>R[x]&lt;-M[PS+s_e(imm)]</t>
-  </si>
-  <si>
     <t>sw</t>
   </si>
   <si>
@@ -383,19 +385,21 @@
   </si>
   <si>
     <t>R[z]&lt;-R[x]+R[y]</t>
+  </si>
+  <si>
+    <t>ry</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>R[x]&lt;-M[SP+s_e(imm)]</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -419,355 +423,24 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
-      <charset val="134"/>
+      <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -812,253 +485,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1069,6 +500,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1088,66 +529,91 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1159,7 +625,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="CCE8CF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1437,21 +903,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="3.74166666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.65833333333333" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.18333333333333" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.68333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="5.625" style="2" customWidth="1"/>
     <col min="7" max="13" width="5.625" style="3" customWidth="1"/>
     <col min="14" max="21" width="5.625" style="2" customWidth="1"/>
@@ -1460,19 +925,19 @@
     <col min="24" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="14.25" spans="6:13">
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" ht="14.25" spans="7:21">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.15">
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
@@ -1480,15 +945,15 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
-      <c r="Q3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="7"/>
-    </row>
-    <row r="4" ht="14.25" spans="7:21">
+      <c r="Q3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="11"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -1496,18 +961,18 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="7"/>
-    </row>
-    <row r="5" ht="14.25" spans="3:21">
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="11"/>
+    </row>
+    <row r="5" spans="1:23" ht="67.5" x14ac:dyDescent="0.15">
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1521,27 +986,27 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="5" t="s">
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="5" t="s">
+      <c r="O5" s="10"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="R5" s="6"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="5" t="s">
+      <c r="R5" s="10"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="7"/>
-    </row>
-    <row r="6" ht="14.25" customHeight="1" spans="3:23">
+      <c r="U5" s="11"/>
+    </row>
+    <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1549,30 +1014,30 @@
         <v>11</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="5" t="s">
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="5" t="s">
+      <c r="O6" s="10"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="7"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="11"/>
       <c r="V6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1580,7 +1045,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1" spans="3:21">
+    <row r="7" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1633,7 +1098,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1698,7 +1163,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1747,9 +1212,12 @@
       <c r="Q9" s="2">
         <v>0</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="R9" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
       <c r="V9" s="2" t="s">
         <v>43</v>
       </c>
@@ -1757,7 +1225,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>45</v>
       </c>
@@ -1785,12 +1253,21 @@
       <c r="J10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
       <c r="V10" s="2" t="s">
         <v>48</v>
       </c>
@@ -1798,7 +1275,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>50</v>
       </c>
@@ -1826,9 +1303,11 @@
       <c r="J11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="K11" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
       <c r="N11" s="2">
         <v>0</v>
       </c>
@@ -1857,7 +1336,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>53</v>
       </c>
@@ -1885,9 +1364,11 @@
       <c r="J12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
       <c r="N12" s="2">
         <v>0</v>
       </c>
@@ -1916,7 +1397,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -1944,9 +1425,11 @@
       <c r="J13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
       <c r="N13" s="2">
         <v>0</v>
       </c>
@@ -1975,7 +1458,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>58</v>
       </c>
@@ -2003,12 +1486,16 @@
       <c r="J14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N14" s="2" t="s">
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
       <c r="Q14" s="2">
         <v>0</v>
       </c>
@@ -2028,7 +1515,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
@@ -2065,9 +1552,11 @@
       <c r="M15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="N15" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
       <c r="Q15" s="2">
         <v>0</v>
       </c>
@@ -2087,7 +1576,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2115,22 +1604,24 @@
       <c r="J16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
       <c r="W16" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:23">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>67</v>
       </c>
@@ -2158,17 +1649,26 @@
       <c r="J17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
       <c r="W17" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:23">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -2196,17 +1696,26 @@
       <c r="J18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
       <c r="W18" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:23">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>71</v>
       </c>
@@ -2243,14 +1752,21 @@
       <c r="M19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="N19" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
       <c r="W19" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:23">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>73</v>
       </c>
@@ -2278,9 +1794,11 @@
       <c r="J20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="15" t="s">
         <v>6</v>
       </c>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
       <c r="N20" s="2">
         <v>0</v>
       </c>
@@ -2309,7 +1827,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>75</v>
       </c>
@@ -2337,20 +1855,28 @@
       <c r="J21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N21" s="2" t="s">
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
       <c r="W21" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>77</v>
       </c>
@@ -2378,19 +1904,28 @@
       <c r="J22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
       <c r="W22" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A23" s="1" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23">
-      <c r="A23" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>35</v>
@@ -2416,22 +1951,30 @@
       <c r="J23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
       <c r="W23" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23">
-      <c r="A24" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>35</v>
@@ -2457,25 +2000,34 @@
       <c r="J24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K24" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
       <c r="W24" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A25" s="1" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23">
-      <c r="A25" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>61</v>
@@ -2495,12 +2047,16 @@
       <c r="J25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="3" t="s">
+      <c r="K25" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
       <c r="Q25" s="2">
         <v>0</v>
       </c>
@@ -2517,18 +2073,18 @@
         <v>0</v>
       </c>
       <c r="W25" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A26" s="1" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23">
-      <c r="A26" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>47</v>
@@ -2548,25 +2104,34 @@
       <c r="J26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N26" s="2" t="s">
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
+      <c r="N26" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
       <c r="W26" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A27" s="1" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23">
-      <c r="A27" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>61</v>
@@ -2586,12 +2151,16 @@
       <c r="J27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K27" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
       <c r="Q27" s="2">
         <v>0</v>
       </c>
@@ -2608,18 +2177,18 @@
         <v>0</v>
       </c>
       <c r="W27" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A28" s="1" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23">
-      <c r="A28" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>61</v>
@@ -2639,12 +2208,16 @@
       <c r="J28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="K28" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
       <c r="Q28" s="2">
         <v>0</v>
       </c>
@@ -2661,18 +2234,18 @@
         <v>1</v>
       </c>
       <c r="W28" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A29" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23">
-      <c r="A29" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>61</v>
@@ -2692,12 +2265,16 @@
       <c r="J29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N29" s="2" t="s">
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
       <c r="Q29" s="2">
         <v>0</v>
       </c>
@@ -2714,72 +2291,78 @@
         <v>1</v>
       </c>
       <c r="W29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="30" ht="15" spans="1:23">
-      <c r="A30" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="2">
+        <v>0</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R30" s="8"/>
+      <c r="S30" s="8"/>
+      <c r="T30" s="2">
+        <v>0</v>
+      </c>
+      <c r="U30" s="2">
+        <v>0</v>
+      </c>
+      <c r="V30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="2">
-        <v>0</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="T30" s="2">
-        <v>0</v>
-      </c>
-      <c r="U30" s="2">
-        <v>0</v>
-      </c>
-      <c r="V30" s="12" t="s">
+      <c r="W30" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="W30" s="13" t="s">
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A31" s="1" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23">
-      <c r="A31" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="F31" s="2">
         <v>0</v>
       </c>
@@ -2795,15 +2378,21 @@
       <c r="J31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K31" s="3" t="s">
+      <c r="K31" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N31" s="2" t="s">
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
+      <c r="N31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q31" s="2" t="s">
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="R31" s="8"/>
+      <c r="S31" s="8"/>
       <c r="T31" s="2">
         <v>1</v>
       </c>
@@ -2811,25 +2400,25 @@
         <v>1</v>
       </c>
       <c r="V31" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="W31" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="W31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A32" s="1" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23">
-      <c r="A32" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E32" s="1" t="s">
-        <v>96</v>
-      </c>
       <c r="F32" s="2">
         <v>0</v>
       </c>
@@ -2845,15 +2434,21 @@
       <c r="J32" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="K32" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N32" s="2" t="s">
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q32" s="2" t="s">
+      <c r="O32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="R32" s="8"/>
+      <c r="S32" s="8"/>
       <c r="T32" s="2">
         <v>1</v>
       </c>
@@ -2861,21 +2456,21 @@
         <v>0</v>
       </c>
       <c r="V32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="W32" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="W32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="33" ht="15" spans="1:23">
-      <c r="A33" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>61</v>
@@ -2916,69 +2511,75 @@
       <c r="U33" s="2">
         <v>0</v>
       </c>
-      <c r="V33" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="W33" s="13" t="s">
+      <c r="V33" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A34" s="1" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23">
-      <c r="A34" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="Q34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="R34" s="8"/>
+      <c r="S34" s="8"/>
+      <c r="T34" s="2">
+        <v>1</v>
+      </c>
+      <c r="U34" s="2">
+        <v>1</v>
+      </c>
+      <c r="W34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="T34" s="2">
-        <v>1</v>
-      </c>
-      <c r="U34" s="2">
-        <v>1</v>
-      </c>
-      <c r="W34" s="1" t="s">
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A35" s="1" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23">
-      <c r="A35" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>47</v>
@@ -2998,32 +2599,34 @@
       <c r="J35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K35" s="3" t="s">
+      <c r="K35" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N35" s="3" t="s">
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="O35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="15"/>
+      <c r="S35" s="15"/>
+      <c r="T35" s="15"/>
+      <c r="U35" s="15"/>
       <c r="W35" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A36" s="1" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23">
-      <c r="A36" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>41</v>
@@ -3043,31 +2646,38 @@
       <c r="J36" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K36" s="3" t="s">
+      <c r="K36" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N36" s="2" t="s">
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="8" t="s">
         <v>7</v>
       </c>
+      <c r="O36" s="8"/>
+      <c r="P36" s="8"/>
       <c r="Q36" s="2">
         <v>0</v>
       </c>
-      <c r="R36" s="2" t="s">
+      <c r="R36" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="S36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="U36" s="8"/>
       <c r="W36" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A37" s="1" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="37" spans="1:23">
-      <c r="A37" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>47</v>
@@ -3096,26 +2706,33 @@
       <c r="M37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N37" s="2" t="s">
+      <c r="N37" s="8" t="s">
         <v>42</v>
       </c>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="8"/>
+      <c r="R37" s="8"/>
+      <c r="S37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="U37" s="8"/>
       <c r="W37" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A38" s="1" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23">
-      <c r="A38" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>109</v>
-      </c>
       <c r="F38" s="2">
         <v>1</v>
       </c>
@@ -3131,15 +2748,21 @@
       <c r="J38" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="K38" s="3" t="s">
+      <c r="K38" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="N38" s="2" t="s">
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q38" s="2" t="s">
+      <c r="O38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="R38" s="8"/>
+      <c r="S38" s="8"/>
       <c r="T38" s="2">
         <v>0</v>
       </c>
@@ -3147,16 +2770,77 @@
         <v>1</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="11:13">
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="68">
+    <mergeCell ref="N37:U37"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="N38:P38"/>
+    <mergeCell ref="Q38:S38"/>
+    <mergeCell ref="K35:M35"/>
+    <mergeCell ref="N35:U35"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="N36:P36"/>
+    <mergeCell ref="R36:U36"/>
+    <mergeCell ref="K32:M32"/>
+    <mergeCell ref="N32:P32"/>
+    <mergeCell ref="Q32:S32"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="Q34:S34"/>
+    <mergeCell ref="K30:M30"/>
+    <mergeCell ref="N30:P30"/>
+    <mergeCell ref="Q30:S30"/>
+    <mergeCell ref="K31:M31"/>
+    <mergeCell ref="N31:P31"/>
+    <mergeCell ref="Q31:S31"/>
+    <mergeCell ref="K27:M27"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="N28:P28"/>
+    <mergeCell ref="K29:M29"/>
+    <mergeCell ref="N29:P29"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:U24"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:U26"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:U22"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="N23:P23"/>
+    <mergeCell ref="Q23:U23"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="N18:U18"/>
+    <mergeCell ref="N19:U19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q21:U21"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="N15:P15"/>
+    <mergeCell ref="K16:U16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="N17:U17"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="N10:U10"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
+    <mergeCell ref="Q6:U6"/>
+    <mergeCell ref="R9:U9"/>
     <mergeCell ref="F2:M2"/>
     <mergeCell ref="Q3:U3"/>
     <mergeCell ref="N4:U4"/>
@@ -3164,70 +2848,9 @@
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="Q5:S5"/>
     <mergeCell ref="T5:U5"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="Q6:U6"/>
-    <mergeCell ref="R9:U9"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="N10:U10"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="N15:P15"/>
-    <mergeCell ref="K16:U16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="N17:U17"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="N18:U18"/>
-    <mergeCell ref="N19:U19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q21:U21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:U22"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="N23:P23"/>
-    <mergeCell ref="Q23:U23"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:U24"/>
-    <mergeCell ref="K25:M25"/>
-    <mergeCell ref="N25:P25"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:U26"/>
-    <mergeCell ref="K27:M27"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="K28:M28"/>
-    <mergeCell ref="N28:P28"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N29:P29"/>
-    <mergeCell ref="K30:M30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="K31:M31"/>
-    <mergeCell ref="N31:P31"/>
-    <mergeCell ref="Q31:S31"/>
-    <mergeCell ref="K32:M32"/>
-    <mergeCell ref="N32:P32"/>
-    <mergeCell ref="Q32:S32"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="Q34:S34"/>
-    <mergeCell ref="K35:M35"/>
-    <mergeCell ref="N35:U35"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="N36:P36"/>
-    <mergeCell ref="R36:U36"/>
-    <mergeCell ref="N37:U37"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="N38:P38"/>
-    <mergeCell ref="Q38:S38"/>
   </mergeCells>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>